<commit_message>
updated FPGA init procedure updated -- next gen layout
</commit_message>
<xml_diff>
--- a/plug-ins/control/RedPitaya-Support/McBSP-Link-Hardware/MK3-RP-Link/rp-shield-PCBWay-BOM.xlsx
+++ b/plug-ins/control/RedPitaya-Support/McBSP-Link-Hardware/MK3-RP-Link/rp-shield-PCBWay-BOM.xlsx
@@ -236,7 +236,7 @@
     <t xml:space="preserve">2x13 (26pin) RP connector (raspberry pi style stacking header, long) BOTTOM MOUNT!</t>
   </si>
   <si>
-    <t xml:space="preserve">do not populate (BOTTOM MOUNT)</t>
+    <t xml:space="preserve">do not populate</t>
   </si>
   <si>
     <t xml:space="preserve">RP-NTH-RX</t>
@@ -320,6 +320,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -402,7 +403,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -444,23 +445,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -468,10 +453,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,7 +553,7 @@
   <dimension ref="A2:I27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -698,32 +679,32 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
@@ -735,7 +716,7 @@
       <c r="C10" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -768,10 +749,10 @@
       <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -841,7 +822,7 @@
       <c r="A14" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="6" t="n">
@@ -873,7 +854,7 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
@@ -884,20 +865,20 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
@@ -906,7 +887,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
@@ -917,7 +898,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
@@ -928,7 +909,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
@@ -939,7 +920,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
     </row>
@@ -950,42 +931,42 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-    </row>
-    <row r="27" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>